<commit_message>
the collection data complete, record complete
</commit_message>
<xml_diff>
--- a/Collection of Data.xlsx
+++ b/Collection of Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heihe\Desktop\Malaysia-Legal-Doc-Classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF100C93-EE8F-4F0E-9C7F-974C6890EED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181974B7-6D0A-4EBE-B967-BEA4517D9560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{B522ABC2-402C-4421-88A0-6A5C2D341CC7}"/>
+    <workbookView xWindow="696" yWindow="804" windowWidth="17280" windowHeight="11016" xr2:uid="{B522ABC2-402C-4421-88A0-6A5C2D341CC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
   <si>
     <t>label</t>
   </si>
@@ -43,9 +43,6 @@
     <t>abetment</t>
   </si>
   <si>
-    <t>Testing DATA - last 10 years</t>
-  </si>
-  <si>
     <t>Corruption</t>
   </si>
   <si>
@@ -61,22 +58,58 @@
     <t>Dangerous Drugs</t>
   </si>
   <si>
-    <t xml:space="preserve">Defense </t>
-  </si>
-  <si>
     <t>Firearms</t>
   </si>
   <si>
-    <t>Security Offences</t>
-  </si>
-  <si>
     <t>Sendition</t>
   </si>
   <si>
-    <t>Total data</t>
-  </si>
-  <si>
-    <t>Training DATA - last 10 years</t>
+    <t>Rape</t>
+  </si>
+  <si>
+    <t>Murder</t>
+  </si>
+  <si>
+    <t>Total data - 00's</t>
+  </si>
+  <si>
+    <t>Training DATA -00's</t>
+  </si>
+  <si>
+    <t>Testing DATA - 00's</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Defence </t>
+  </si>
+  <si>
+    <t>Offences</t>
+  </si>
+  <si>
+    <t>12 labels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Range: </t>
+  </si>
+  <si>
+    <t>00's</t>
+  </si>
+  <si>
+    <t>Training data = 45</t>
+  </si>
+  <si>
+    <t>Testing data = 35</t>
+  </si>
+  <si>
+    <t>Challenge - one file two label!!!</t>
+  </si>
+  <si>
+    <t>LNS_2016_1_1067_psb.pdf</t>
+  </si>
+  <si>
+    <t>Two labelling</t>
+  </si>
+  <si>
+    <t>firearms and common intention</t>
   </si>
 </sst>
 </file>
@@ -100,12 +133,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -120,9 +171,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADB7DB2D-06F1-43F1-9934-41865AF0A626}">
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -449,244 +503,311 @@
     <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5" s="4">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
+      <c r="B6">
+        <v>29</v>
+      </c>
+      <c r="C6" s="4">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="C7" s="4">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B8">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
       <c r="B9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="C9" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B10">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="C10" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11">
+        <v>79</v>
+      </c>
+      <c r="C11" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>16</v>
+      </c>
+      <c r="C12" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B13" s="1">
-        <f>SUM(B3:B12)</f>
-        <v>107</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="C13" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B15" s="1">
+        <f>SUM(B3:B14)</f>
+        <v>237</v>
+      </c>
+      <c r="C15" s="1">
+        <f>SUM(C3:C14)</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>2</v>
-      </c>
-      <c r="B16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>5</v>
       </c>
       <c r="B18">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>6</v>
       </c>
-      <c r="B19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="B20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>7</v>
       </c>
-      <c r="B20">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="B22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>8</v>
       </c>
-      <c r="B21">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="B24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26">
+        <v>5</v>
+      </c>
+      <c r="F26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="F27" t="s">
+        <v>24</v>
+      </c>
+      <c r="G27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>9</v>
       </c>
-      <c r="B22">
+      <c r="B29">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B26" s="1">
-        <f>SUM(B16:B25)</f>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>2</v>
-      </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>5</v>
-      </c>
-      <c r="B31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>6</v>
-      </c>
-      <c r="B32">
-        <v>5</v>
+      <c r="F29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B30" s="1">
+        <f>SUM(B18:B29)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B33">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B34">
         <v>5</v>
@@ -694,43 +815,94 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B35">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B36">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B38">
         <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B39" s="1">
-        <f>SUM(B29:B38)</f>
-        <v>30</v>
+      <c r="A39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>10</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B45" s="1">
+        <f>SUM(B33:B44)</f>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B14">
+    <sortCondition ref="A3:A14"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>